<commit_message>
SE REALIZA CORRECCION AL DIAGRAMA DE CLASES Y SE ANEXA CARPETA CON DISTRIBUCION DEL SPRINT 3
</commit_message>
<xml_diff>
--- a/SPRINT2/FORMATO SEGUIMIENTO-SPRINT2.xlsx
+++ b/SPRINT2/FORMATO SEGUIMIENTO-SPRINT2.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/SPRINT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C884A35F-0EE9-9746-8FBF-59E3ABF38601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D159E2A-7F20-BC4B-8BCA-3B69DBE373A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME SPRINT" sheetId="12" r:id="rId1"/>
-    <sheet name="REUNION 02-09-2022" sheetId="21" r:id="rId2"/>
-    <sheet name="REUNION 01-09-2022" sheetId="20" r:id="rId3"/>
-    <sheet name="REUNION 30-08-2022" sheetId="18" r:id="rId4"/>
-    <sheet name="REUNION 29-08-2022" sheetId="17" r:id="rId5"/>
-    <sheet name="DISTRIBUCION 28-08-2022" sheetId="16" r:id="rId6"/>
+    <sheet name="REUNION 04-09-2022" sheetId="22" r:id="rId2"/>
+    <sheet name="REUNION 02-09-2022" sheetId="21" r:id="rId3"/>
+    <sheet name="TUTORIA 01-09-2022" sheetId="20" r:id="rId4"/>
+    <sheet name="REUNION 30-08-2022" sheetId="18" r:id="rId5"/>
+    <sheet name="REUNION 29-08-2022" sheetId="17" r:id="rId6"/>
+    <sheet name="DISTRIBUCION 28-08-2022" sheetId="16" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -204,6 +205,12 @@
   </si>
   <si>
     <t>TUTORIA</t>
+  </si>
+  <si>
+    <t>SEGUIMIENTO 4</t>
+  </si>
+  <si>
+    <t>POSPUESTO</t>
   </si>
 </sst>
 </file>
@@ -714,6 +721,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,18 +754,72 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,48 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -816,22 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -839,440 +846,30 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="109">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1293,7 +890,95 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1323,7 +1008,95 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1353,9 +1126,98 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1365,15 +1227,107 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1383,15 +1337,107 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1401,28 +1447,99 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1689,19 +1806,86 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>36690</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3084690</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE5908D7-37AB-3447-98FC-73CD2FFE6B30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10817579" y="11994445"/>
+          <a:ext cx="3048000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B5ACF9CC-BD44-E14E-AAC2-63AD590D4699}" name="Reunion37" displayName="Reunion37" ref="A1:F7" totalsRowCount="1" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A853B00-DDD4-4B4D-B617-507F5D51678B}" name="Reunion372" displayName="Reunion372" ref="A1:F7" totalsRowCount="1" headerRowDxfId="100">
   <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{591DE6F2-A06B-9D46-BE8A-79DEEF8BCAE8}" name="ID" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{DC998DB0-3CD2-A34E-9F31-5D66476C382A}" name="VALOR" totalsRowDxfId="45" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{CB8B5BB5-79F1-254A-AC9E-DA110767FA59}" name="ACTIVIDAD" dataDxfId="53" totalsRowDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{49F7F14D-51A5-2E4E-9303-F4F422ECD62B}" name="RESPONSABLE" dataDxfId="52" totalsRowDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{4BE6F1D9-6515-574D-B6FA-CE2A1EA2C3FC}" name="ESTADO" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{39C1ECF6-729A-9444-8510-FDF8CFBC1B2E}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="42" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{B8842E4A-CC18-D34C-9B00-B0139091736A}" name="ID" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{184E2062-8377-B54A-B65C-8574903F6D2F}" name="VALOR" totalsRowDxfId="98" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{2DD46EB5-6AE4-AB49-8571-ED44C274E61B}" name="ACTIVIDAD" dataDxfId="97" totalsRowDxfId="96"/>
+    <tableColumn id="6" xr3:uid="{9C748491-42D9-5642-97EE-AE9AC44D59D2}" name="RESPONSABLE" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{E7546DE8-8B7E-0547-A3EA-D58EACD00331}" name="ESTADO" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{E673E466-56E9-7941-A3A3-1AF69B8ACCBB}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B5ACF9CC-BD44-E14E-AAC2-63AD590D4699}" name="Reunion37" displayName="Reunion37" ref="A1:F7" totalsRowCount="1" headerRowDxfId="82">
+  <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{591DE6F2-A06B-9D46-BE8A-79DEEF8BCAE8}" name="ID" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{DC998DB0-3CD2-A34E-9F31-5D66476C382A}" name="VALOR" totalsRowDxfId="80" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{CB8B5BB5-79F1-254A-AC9E-DA110767FA59}" name="ACTIVIDAD" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{49F7F14D-51A5-2E4E-9303-F4F422ECD62B}" name="RESPONSABLE" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{4BE6F1D9-6515-574D-B6FA-CE2A1EA2C3FC}" name="ESTADO" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{39C1ECF6-729A-9444-8510-FDF8CFBC1B2E}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="74" totalsRowDxfId="73" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Reunion37[[#This Row],[ESTADO]]="HECHO",Reunion37[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1709,16 +1893,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70A4F03D-6E61-E84D-BEFA-21C76986CDAA}" name="Reunion3" displayName="Reunion3" ref="A1:F7" totalsRowCount="1" headerRowDxfId="90">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70A4F03D-6E61-E84D-BEFA-21C76986CDAA}" name="Reunion3" displayName="Reunion3" ref="A1:F7" totalsRowCount="1" headerRowDxfId="64">
   <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1B44A4FC-9761-4840-B362-B0B67D46979D}" name="ID" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{BDDC95EC-E4E2-9548-BB7C-B4B36749B07D}" name="VALOR" totalsRowDxfId="49" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{7FC7D9C6-9373-1D43-8BC0-9693E8633ADC}" name="ACTIVIDAD" dataDxfId="88" totalsRowDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{5A31B5C8-136A-C54E-8EC8-BD9E610E161C}" name="RESPONSABLE" dataDxfId="87" totalsRowDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{ADB9CF60-B088-1546-A904-459333E6AE8A}" name="ESTADO" dataDxfId="86"/>
-    <tableColumn id="4" xr3:uid="{C4728F1A-A765-704A-88C1-4AD6C63B8640}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="46" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{1B44A4FC-9761-4840-B362-B0B67D46979D}" name="ID" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BDDC95EC-E4E2-9548-BB7C-B4B36749B07D}" name="VALOR" totalsRowDxfId="62" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{7FC7D9C6-9373-1D43-8BC0-9693E8633ADC}" name="ACTIVIDAD" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{5A31B5C8-136A-C54E-8EC8-BD9E610E161C}" name="RESPONSABLE" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{ADB9CF60-B088-1546-A904-459333E6AE8A}" name="ESTADO" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{C4728F1A-A765-704A-88C1-4AD6C63B8640}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1726,16 +1910,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E87A051E-30B6-6543-A351-182DB28CD0DF}" name="Reunion2" displayName="Reunion2" ref="A1:F7" totalsRowCount="1" headerRowDxfId="84">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E87A051E-30B6-6543-A351-182DB28CD0DF}" name="Reunion2" displayName="Reunion2" ref="A1:F7" totalsRowCount="1" headerRowDxfId="46">
   <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5D8DDD81-A049-7A4D-8F63-C52AD0FAF0B3}" name="ID" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{3642A657-9D7D-C843-8078-ABE3CDE26154}" name="VALOR" dataDxfId="66" totalsRowDxfId="65" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{E2BA7776-5644-E542-A744-A0A32EDA687D}" name="ACTIVIDAD" dataDxfId="82" totalsRowDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{52157B39-F9FA-A748-946C-FD256BC7430D}" name="RESPONSABLE" dataDxfId="81" totalsRowDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{00E318AC-2DC1-4843-8BF7-20A1128848C1}" name="ESTADO" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{8E2B9799-F11A-334F-8747-54B12B2ED139}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="62" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{5D8DDD81-A049-7A4D-8F63-C52AD0FAF0B3}" name="ID" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{3642A657-9D7D-C843-8078-ABE3CDE26154}" name="VALOR" dataDxfId="44" totalsRowDxfId="43" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{E2BA7776-5644-E542-A744-A0A32EDA687D}" name="ACTIVIDAD" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{52157B39-F9FA-A748-946C-FD256BC7430D}" name="RESPONSABLE" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00E318AC-2DC1-4843-8BF7-20A1128848C1}" name="ESTADO" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{8E2B9799-F11A-334F-8747-54B12B2ED139}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1743,16 +1927,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6335B5E8-8C68-9849-B638-16F4C68A443C}" name="Reunion1" displayName="Reunion1" ref="A1:F7" totalsRowCount="1" headerRowDxfId="78">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6335B5E8-8C68-9849-B638-16F4C68A443C}" name="Reunion1" displayName="Reunion1" ref="A1:F7" totalsRowCount="1" headerRowDxfId="28">
   <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0A7A4574-5A4E-AC4E-8215-EEFA2C8E799F}" name="ID" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{A9ECA477-E218-7B40-B14E-C7ADB0FD3FAD}" name="VALOR" dataDxfId="61" totalsRowDxfId="60" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{37C02F32-5CEE-904D-8C20-6A8783C18240}" name="ACTIVIDAD" dataDxfId="76" totalsRowDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{B98B6820-93D5-5941-A278-D1F0E116E71F}" name="RESPONSABLE" dataDxfId="75" totalsRowDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{C7834CA5-7D54-DB4A-AAB9-5FFA6FA1E74E}" name="ESTADO" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{1B286B3A-1A7F-F94F-9F0F-5AD681567A93}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="57" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{0A7A4574-5A4E-AC4E-8215-EEFA2C8E799F}" name="ID" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{A9ECA477-E218-7B40-B14E-C7ADB0FD3FAD}" name="VALOR" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{37C02F32-5CEE-904D-8C20-6A8783C18240}" name="ACTIVIDAD" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B98B6820-93D5-5941-A278-D1F0E116E71F}" name="RESPONSABLE" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{C7834CA5-7D54-DB4A-AAB9-5FFA6FA1E74E}" name="ESTADO" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{1B286B3A-1A7F-F94F-9F0F-5AD681567A93}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1760,16 +1944,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DD23BDD-0C6B-9546-BC60-2B699E1DBBD8}" name="Distribucion" displayName="Distribucion" ref="A1:F7" totalsRowCount="1" headerRowDxfId="72">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DD23BDD-0C6B-9546-BC60-2B699E1DBBD8}" name="Distribucion" displayName="Distribucion" ref="A1:F7" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:F6" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{73C66182-65A3-1E48-B252-9CA7D86615F7}" name="ID" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{38DA5FEB-20A4-EE4A-9128-74DFB57CD030}" name="VALOR" dataDxfId="56" totalsRowDxfId="3" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{71F59E7D-B04C-E04A-9AFF-C00FB83CFA4D}" name="ACTIVIDAD" dataDxfId="70" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{DA1AAC07-60AB-BF43-8A94-8802E652232B}" name="RESPONSABLE" dataDxfId="69" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{8C839BBF-3DCE-0441-99C9-D9C276414CC3}" name="ESTADO" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{B9AFE5A4-3815-444E-84B9-842AFAFA53BB}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{73C66182-65A3-1E48-B252-9CA7D86615F7}" name="ID" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{38DA5FEB-20A4-EE4A-9128-74DFB57CD030}" name="VALOR" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{71F59E7D-B04C-E04A-9AFF-C00FB83CFA4D}" name="ACTIVIDAD" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{DA1AAC07-60AB-BF43-8A94-8802E652232B}" name="RESPONSABLE" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8C839BBF-3DCE-0441-99C9-D9C276414CC3}" name="ESTADO" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B9AFE5A4-3815-444E-84B9-842AFAFA53BB}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2040,10 +2224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30953C18-D402-474E-9F52-63E7C872EAD8}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2061,7 +2245,7 @@
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -2073,258 +2257,258 @@
       <c r="E1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="52">
         <v>44801</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="42"/>
-      <c r="G2" s="25" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="40"/>
+      <c r="G2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="43"/>
-      <c r="G3" s="25" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="41"/>
+      <c r="G3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="43"/>
-      <c r="G4" s="25" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="41"/>
+      <c r="G4" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="43"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="41"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="43"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="41"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="44"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="52">
         <v>44802</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="43"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="41"/>
       <c r="G9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="43"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="41"/>
       <c r="G10" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="30">
         <v>44805</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="43"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="41"/>
       <c r="G11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="43"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="44"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="59">
+      <c r="B14" s="52">
         <v>44803</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="42"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="43"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="43"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="41"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="43"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="41"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="43"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="44"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="59">
+      <c r="B20" s="52">
         <v>37500</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="40"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="43"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="41"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="43"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="43"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="43"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="44"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="42"/>
       <c r="G25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2332,59 +2516,118 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="59">
+      <c r="B26" s="52">
         <v>44806</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="42"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="40"/>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="43"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="43"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="41"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="43"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="41"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="43"/>
+      <c r="A30" s="56"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="41"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="42"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="52">
+        <v>44808</v>
+      </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="40"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="56"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="56"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="41"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="56"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="56"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="57"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="B26:B31"/>
+  <mergeCells count="63">
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
     <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="E26:E31"/>
@@ -2392,7 +2635,6 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A20:A25"/>
     <mergeCell ref="E20:E25"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -2400,11 +2642,8 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A2:A7"/>
     <mergeCell ref="E2:E7"/>
-    <mergeCell ref="A8:A13"/>
     <mergeCell ref="E8:E13"/>
-    <mergeCell ref="A14:A19"/>
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
@@ -2440,11 +2679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726DD20D-2421-5549-8FE2-FCCDD1F6E994}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077739A0-7BE1-0545-B3E1-4184E488F9FC}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2494,6 +2733,298 @@
         <v>45</v>
       </c>
       <c r="F2" s="5">
+        <f>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="5">
+        <f>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f>IF(Reunion372[[#This Row],[ESTADO]]="HECHO",Reunion372[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="F7" s="6">
+        <f>SUBTOTAL(109,Reunion372[PROGRESO])</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <f>COUNTIF(Reunion372[ESTADO],"HACER")</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
+        <f>COUNTIF(Reunion372[ESTADO],"HACIENDO")</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="20">
+        <v>1</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2">
+        <f>COUNTIF(Reunion372[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="20">
+        <v>2</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <f>COUNTIF(Reunion372[ESTADO],"HECHO")</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="20">
+        <v>3</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2">
+        <f>COUNTIF(Reunion372[ESTADO],"POSPUESTO")</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="20">
+        <v>4</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E6">
+    <cfRule type="expression" dxfId="108" priority="1" stopIfTrue="1">
+      <formula>($E2="POSPUESTO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="5" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="6" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="7" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="8" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="103" priority="2" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="3" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{AD468895-1638-2B4D-9E3B-B811CC185D5A}">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{5C9A56C2-1C01-3749-AE04-C75CBF302617}">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726DD20D-2421-5549-8FE2-FCCDD1F6E994}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="9" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5">
         <f>IF(Reunion37[[#This Row],[ESTADO]]="HECHO",Reunion37[[#This Row],[VALOR]]," ")</f>
         <v>0.5</v>
       </c>
@@ -2688,31 +3219,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="1" stopIfTrue="1">
       <formula>($E2="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="5" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="6" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="7" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="8" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="36" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="84" priority="3" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2731,12 +3262,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19891FED-D2D3-7A41-B50E-8194D783E769}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2980,31 +3511,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="expression" dxfId="33" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="1" stopIfTrue="1">
       <formula>($E2="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="5" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="6" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="7" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="8" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="3" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3023,12 +3554,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB2A483-9E80-6B40-A127-ED09E1519ABA}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3272,31 +3803,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="1" stopIfTrue="1">
       <formula>($E2="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="6" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="7" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="8" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="3" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3315,12 +3846,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A44FC23-7A3E-0C46-A9BD-B97D74A269B3}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3564,28 +4095,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3604,12 +4135,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB54409-1CE7-2449-8423-28A02DE4E2D1}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3843,28 +4374,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>